<commit_message>
four pages, legible figures
</commit_message>
<xml_diff>
--- a/StmtType.xlsx
+++ b/StmtType.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chupanw/Box Sync/Courses/15-819O/hw1b/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26122"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="11900" yWindow="3280" windowWidth="28800" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -719,11 +714,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2093323792"/>
-        <c:axId val="-2093320304"/>
+        <c:axId val="2141036232"/>
+        <c:axId val="2141039912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2093323792"/>
+        <c:axId val="2141036232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,7 +761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093320304"/>
+        <c:crossAx val="2141039912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -774,7 +769,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093320304"/>
+        <c:axId val="2141039912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -825,7 +820,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093323792"/>
+        <c:crossAx val="2141036232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -921,7 +916,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0634655355420398"/>
+          <c:y val="0.0324846575996182"/>
+          <c:w val="0.827417298138308"/>
+          <c:h val="0.749757227261944"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -965,12 +970,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1179,12 +1181,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1393,12 +1392,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1578,11 +1574,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2090585296"/>
-        <c:axId val="-2090581712"/>
+        <c:axId val="2143446024"/>
+        <c:axId val="2143449800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2090585296"/>
+        <c:axId val="2143446024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,12 +1606,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:effectLst>
                   <a:outerShdw blurRad="50800" dist="50800" dir="5400000" sx="1000" sy="1000" algn="ctr" rotWithShape="0">
@@ -1632,7 +1625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090581712"/>
+        <c:crossAx val="2143449800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1640,7 +1633,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2090581712"/>
+        <c:axId val="2143449800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1661,7 +1654,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1677,12 +1670,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1692,7 +1682,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090585296"/>
+        <c:crossAx val="2143446024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1705,8 +1695,17 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.900285901272273"/>
+          <c:y val="0.260771133880862"/>
+          <c:w val="0.0903047939708007"/>
+          <c:h val="0.214469210000113"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1720,12 +1719,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2898,15 +2894,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>158750</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2971,7 +2967,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -3006,7 +3002,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -3183,7 +3179,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3193,13 +3189,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -3210,7 +3206,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3228,7 +3224,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3246,7 +3242,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3264,7 +3260,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3282,7 +3278,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3300,7 +3296,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3318,7 +3314,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3336,7 +3332,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3354,7 +3350,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3372,7 +3368,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3390,7 +3386,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3408,7 +3404,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -3426,7 +3422,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3444,7 +3440,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3462,7 +3458,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3480,7 +3476,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3498,7 +3494,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3516,7 +3512,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3534,7 +3530,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3552,7 +3548,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -3563,7 +3559,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -3580,7 +3576,7 @@
         <v>6.3489518652905157E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -3601,7 +3597,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -3622,7 +3618,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -3643,7 +3639,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -3664,7 +3660,7 @@
       <c r="J28" s="3"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -3685,7 +3681,7 @@
       <c r="J29" s="3"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -3706,7 +3702,7 @@
       <c r="J30" s="3"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -3727,7 +3723,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -3748,7 +3744,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -3769,7 +3765,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -3790,7 +3786,7 @@
       <c r="J34" s="3"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -3811,7 +3807,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -3832,7 +3828,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -3853,7 +3849,7 @@
       <c r="J37" s="3"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -3874,7 +3870,7 @@
       <c r="J38" s="3"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3895,7 +3891,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -3916,7 +3912,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -3937,7 +3933,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -3958,7 +3954,7 @@
       <c r="J42" s="3"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="I43" s="2"/>
       <c r="J43" s="3"/>
       <c r="K43" s="4"/>
@@ -3966,5 +3962,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Used patterns to distinguish bars in StmtType.png
</commit_message>
<xml_diff>
--- a/StmtType.xlsx
+++ b/StmtType.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chupanw/Projects/Papers/MSR-Challenge-2016/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11900" yWindow="3280" windowWidth="28800" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -200,6 +205,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -714,11 +720,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2141036232"/>
-        <c:axId val="2141039912"/>
+        <c:axId val="-2078639008"/>
+        <c:axId val="-2070844016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2141036232"/>
+        <c:axId val="-2078639008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,7 +767,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141039912"/>
+        <c:crossAx val="-2070844016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -769,7 +775,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141039912"/>
+        <c:axId val="-2070844016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -820,7 +826,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141036232"/>
+        <c:crossAx val="-2078639008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -834,6 +840,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -946,9 +953,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="089B77"/>
-            </a:solidFill>
+            <a:pattFill prst="wdDnDiag">
+              <a:fgClr>
+                <a:srgbClr val="089B77"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1157,9 +1169,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="DB6200"/>
-            </a:solidFill>
+            <a:pattFill prst="pct90">
+              <a:fgClr>
+                <a:srgbClr val="DB6200"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1368,9 +1385,14 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="7573B4"/>
-            </a:solidFill>
+            <a:pattFill prst="wdUpDiag">
+              <a:fgClr>
+                <a:srgbClr val="7573B4"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1574,11 +1596,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2143446024"/>
-        <c:axId val="2143449800"/>
+        <c:axId val="-2069984176"/>
+        <c:axId val="-2069980640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2143446024"/>
+        <c:axId val="-2069984176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1625,7 +1647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143449800"/>
+        <c:crossAx val="-2069980640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1633,7 +1655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143449800"/>
+        <c:axId val="-2069980640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1682,7 +1704,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143446024"/>
+        <c:crossAx val="-2069984176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3179,7 +3201,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3189,13 +3211,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="F27" zoomScale="156" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -3206,7 +3228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3224,7 +3246,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3242,7 +3264,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3260,7 +3282,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3278,7 +3300,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3296,7 +3318,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3314,7 +3336,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3332,7 +3354,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3350,7 +3372,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3368,7 +3390,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3386,7 +3408,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3404,7 +3426,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -3422,7 +3444,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3440,7 +3462,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3458,7 +3480,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3476,7 +3498,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3494,7 +3516,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3512,7 +3534,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3530,7 +3552,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3548,7 +3570,7 @@
         <v>4590679</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -3559,7 +3581,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -3576,7 +3598,7 @@
         <v>6.3489518652905157E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -3597,7 +3619,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -3618,7 +3640,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -3639,7 +3661,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -3660,7 +3682,7 @@
       <c r="J28" s="3"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -3681,7 +3703,7 @@
       <c r="J29" s="3"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -3702,7 +3724,7 @@
       <c r="J30" s="3"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -3723,7 +3745,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -3744,7 +3766,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -3765,7 +3787,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -3786,7 +3808,7 @@
       <c r="J34" s="3"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -3807,7 +3829,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -3828,7 +3850,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -3849,7 +3871,7 @@
       <c r="J37" s="3"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -3870,7 +3892,7 @@
       <c r="J38" s="3"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -3891,7 +3913,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -3912,7 +3934,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -3933,7 +3955,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -3954,7 +3976,7 @@
       <c r="J42" s="3"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I43" s="2"/>
       <c r="J43" s="3"/>
       <c r="K43" s="4"/>
@@ -3962,10 +3984,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last commit exceeded 4 pages, fixed now
</commit_message>
<xml_diff>
--- a/StmtType.xlsx
+++ b/StmtType.xlsx
@@ -205,7 +205,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -720,11 +719,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2078639008"/>
-        <c:axId val="-2070844016"/>
+        <c:axId val="-2075877648"/>
+        <c:axId val="-2097425424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2078639008"/>
+        <c:axId val="-2075877648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +766,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2070844016"/>
+        <c:crossAx val="-2097425424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -775,7 +774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2070844016"/>
+        <c:axId val="-2097425424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -826,7 +825,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078639008"/>
+        <c:crossAx val="-2075877648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -840,7 +839,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1596,11 +1594,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2069984176"/>
-        <c:axId val="-2069980640"/>
+        <c:axId val="-2072558064"/>
+        <c:axId val="-2069475632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2069984176"/>
+        <c:axId val="-2072558064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1647,7 +1645,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069980640"/>
+        <c:crossAx val="-2069475632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1655,7 +1653,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2069980640"/>
+        <c:axId val="-2069475632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1704,7 +1702,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069984176"/>
+        <c:crossAx val="-2072558064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1763,12 +1761,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2923,8 +2916,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>166234</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3211,8 +3204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F27" zoomScale="156" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="F30" zoomScale="131" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3983,6 +3976,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>